<commit_message>
update variable description metadata
</commit_message>
<xml_diff>
--- a/Lake Modeling Module_2.0/Variable_Name_Metadata.xlsx
+++ b/Lake Modeling Module_2.0/Variable_Name_Metadata.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KJF\Desktop\R\ProjectEDDIE\LakeModeling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farrellk\Desktop\R\ProjectEDDIE\Lake Modeling Module_2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>File name</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Example</t>
   </si>
   <si>
-    <t>2000-03-02</t>
-  </si>
-  <si>
     <t>met_hourly.csv</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>RelHum</t>
   </si>
   <si>
-    <t xml:space="preserve"> WindSpeed</t>
-  </si>
-  <si>
     <t>Rain</t>
   </si>
   <si>
@@ -98,35 +92,15 @@
     <t>yyyy-mm-dd hh:mm</t>
   </si>
   <si>
-    <t>2000-03-02 12:00</t>
-  </si>
-  <si>
     <t>hourly</t>
   </si>
   <si>
-    <t>Note</t>
-  </si>
-  <si>
     <t>meters/day</t>
   </si>
   <si>
     <t>Convert from mm/d by multiplying by 0.001</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">decimal </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>≥ 0</t>
-    </r>
-  </si>
-  <si>
     <t>meters</t>
   </si>
   <si>
@@ -136,25 +110,22 @@
     <t>%</t>
   </si>
   <si>
-    <r>
-      <t>W/m</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
     <t>m/s</t>
   </si>
   <si>
     <t>Average wind speed 10m above lake surface</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>W/m2</t>
+  </si>
+  <si>
+    <t>WindSpeed</t>
+  </si>
+  <si>
+    <t>decimal ≥ 0</t>
   </si>
 </sst>
 </file>
@@ -162,9 +133,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,13 +152,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -226,7 +190,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -549,7 +513,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection sqref="A1:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,6 +523,7 @@
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -578,7 +543,7 @@
         <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -594,8 +559,8 @@
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>13</v>
+      <c r="E2" s="5">
+        <v>36587</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -606,7 +571,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>11</v>
@@ -615,7 +580,7 @@
         <v>37.799999999999997</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -637,44 +602,50 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="5">
+        <v>36587</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
       <c r="C6" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
       </c>
       <c r="E6">
         <v>-2.5139999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
       </c>
       <c r="E7">
         <v>308.887</v>
@@ -682,10 +653,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>10</v>
@@ -699,13 +670,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
       </c>
       <c r="E9">
         <v>38.619999999999997</v>
@@ -713,53 +687,56 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
       </c>
       <c r="E10">
         <v>1.87</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E11">
         <v>5.9199999999999997E-4</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E12">
         <v>0</v>

</xml_diff>